<commit_message>
fix(tap):it is now loading quesiton from excel sheet
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$54</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$56</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="85">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -53,9 +53,6 @@
     <t xml:space="preserve">a1:9*</t>
   </si>
   <si>
-    <t xml:space="preserve">easy</t>
-  </si>
-  <si>
     <t xml:space="preserve">{a}</t>
   </si>
   <si>
@@ -74,10 +71,10 @@
     <t xml:space="preserve">{a}+{b}+{c}</t>
   </si>
   <si>
-    <t xml:space="preserve">Tape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a10,20,30*?a1:9*?a2:9+30</t>
+    <t xml:space="preserve">tap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a10,20,30*</t>
   </si>
   <si>
     <t xml:space="preserve">a1,2,3*</t>
@@ -152,13 +149,13 @@
     <t xml:space="preserve">drawing</t>
   </si>
   <si>
-    <t xml:space="preserve">arectangle,circle,triangle</t>
+    <t xml:space="preserve">arectangle,circle,triangle*</t>
   </si>
   <si>
     <t xml:space="preserve">direction</t>
   </si>
   <si>
-    <t xml:space="preserve">North,Sourth,West,East</t>
+    <t xml:space="preserve">aNorth,Sourth,West,East*</t>
   </si>
   <si>
     <t xml:space="preserve">touch</t>
@@ -457,10 +454,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,11 +500,11 @@
       <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>30</v>
@@ -515,19 +512,19 @@
     </row>
     <row r="3" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>30</v>
@@ -535,39 +532,39 @@
     </row>
     <row r="4" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>30</v>
@@ -575,79 +572,79 @@
     </row>
     <row r="6" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="E8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="D9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>30</v>
@@ -655,19 +652,19 @@
     </row>
     <row r="10" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>30</v>
@@ -675,19 +672,19 @@
     </row>
     <row r="11" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>30</v>
@@ -695,19 +692,19 @@
     </row>
     <row r="12" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="D12" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>30</v>
@@ -715,19 +712,19 @@
     </row>
     <row r="13" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="D13" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>30</v>
@@ -735,19 +732,19 @@
     </row>
     <row r="14" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>30</v>
@@ -755,19 +752,19 @@
     </row>
     <row r="15" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>30</v>
@@ -775,19 +772,19 @@
     </row>
     <row r="16" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>30</v>
@@ -795,19 +792,19 @@
     </row>
     <row r="17" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>30</v>
@@ -815,19 +812,19 @@
     </row>
     <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="D18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>30</v>
@@ -835,19 +832,19 @@
     </row>
     <row r="19" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>30</v>
@@ -855,19 +852,19 @@
     </row>
     <row r="20" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>30</v>
@@ -875,19 +872,19 @@
     </row>
     <row r="21" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>30</v>
@@ -895,19 +892,19 @@
     </row>
     <row r="22" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>30</v>
@@ -915,19 +912,19 @@
     </row>
     <row r="23" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>30</v>
@@ -935,19 +932,19 @@
     </row>
     <row r="24" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>30</v>
@@ -955,19 +952,19 @@
     </row>
     <row r="25" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>30</v>
@@ -975,19 +972,19 @@
     </row>
     <row r="26" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>30</v>
@@ -995,19 +992,19 @@
     </row>
     <row r="27" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>30</v>
@@ -1015,19 +1012,19 @@
     </row>
     <row r="28" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>30</v>
@@ -1035,19 +1032,19 @@
     </row>
     <row r="29" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>30</v>
@@ -1055,19 +1052,19 @@
     </row>
     <row r="30" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>30</v>
@@ -1075,19 +1072,19 @@
     </row>
     <row r="31" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>30</v>
@@ -1095,10 +1092,10 @@
     </row>
     <row r="32" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>8</v>
@@ -1107,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>30</v>
@@ -1115,10 +1112,10 @@
     </row>
     <row r="33" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>8</v>
@@ -1127,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>30</v>
@@ -1135,10 +1132,10 @@
     </row>
     <row r="34" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>8</v>
@@ -1147,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>30</v>
@@ -1155,10 +1152,10 @@
     </row>
     <row r="35" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>8</v>
@@ -1167,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>30</v>
@@ -1175,10 +1172,10 @@
     </row>
     <row r="36" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>8</v>
@@ -1187,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>30</v>
@@ -1195,10 +1192,10 @@
     </row>
     <row r="37" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>8</v>
@@ -1207,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>30</v>
@@ -1215,10 +1212,10 @@
     </row>
     <row r="38" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>8</v>
@@ -1227,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>30</v>
@@ -1235,10 +1232,10 @@
     </row>
     <row r="39" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>8</v>
@@ -1247,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>30</v>
@@ -1255,10 +1252,10 @@
     </row>
     <row r="40" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>8</v>
@@ -1267,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>30</v>
@@ -1275,10 +1272,10 @@
     </row>
     <row r="41" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>8</v>
@@ -1287,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>30</v>
@@ -1295,10 +1292,10 @@
     </row>
     <row r="42" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>8</v>
@@ -1307,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>30</v>
@@ -1315,10 +1312,10 @@
     </row>
     <row r="43" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>8</v>
@@ -1327,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>30</v>
@@ -1335,10 +1332,10 @@
     </row>
     <row r="44" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>8</v>
@@ -1347,27 +1344,27 @@
         <v>1</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>61</v>
+      <c r="A45" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>30</v>
@@ -1375,119 +1372,119 @@
     </row>
     <row r="46" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="D49" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="5" t="n">
+      <c r="B50" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="0" t="s">
+      <c r="F50" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="B51" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="C51" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>30</v>
@@ -1495,66 +1492,106 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="C54" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="0" t="s">
+      <c r="F54" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="C55" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="F55" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="D56" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D54" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" s="5" t="n">
+      <c r="F56" s="5" t="n">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F54"/>
+  <autoFilter ref="A1:F56"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fix(day) it now loading question from excel sheet
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$56</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="72">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -161,49 +161,10 @@
     <t xml:space="preserve">touch</t>
   </si>
   <si>
-    <t xml:space="preserve">Monday + {a}</t>
-  </si>
-  <si>
     <t xml:space="preserve">day</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuesday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wednesday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thuresday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saturday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunday + {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monday - {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuesday - {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wednesday - {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thuresday - {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friday - {a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saturday -{a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunday - {a}</t>
+    <t xml:space="preserve">a1:5*</t>
   </si>
   <si>
     <t xml:space="preserve">You have ₹{a}, and your friend gives you ₹{b} more.</t>
@@ -454,10 +415,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,10 +1073,10 @@
     </row>
     <row r="33" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>8</v>
@@ -1132,10 +1093,10 @@
     </row>
     <row r="34" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>8</v>
@@ -1152,39 +1113,39 @@
     </row>
     <row r="35" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="C36" s="0" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>30</v>
@@ -1192,406 +1153,197 @@
     </row>
     <row r="37" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="B38" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>30</v>
+      <c r="C38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="0" t="s">
+      <c r="D44" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D55" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F55" s="5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D56" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F56" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F56"/>
+  <autoFilter ref="A1:F45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fix(numberline) it now load question from excel sheets
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$43</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -80,91 +80,109 @@
     <t xml:space="preserve">a1,2,3*</t>
   </si>
   <si>
+    <t xml:space="preserve">mental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*b1:9*c1:9*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} - {b} -{c}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} * {b} *{c}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} /{b} /{c}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*;2/b1:9;2/c2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} + {b} +{c}+{d}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*b1:9*c1:9*d1:9*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} - {b} -{c}+{d}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} * {b} *{c}+{d}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*b1:9*c1:9d1:9*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a} /{b} /{c}/{d}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*;2/b1:9;2/c1:9;2d1*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*;2/b1:9;2/c1:9;2d1:2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a60,30,45,90,120,180,270,360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{a}-{b}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sterio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:9*b1:9*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drawing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arectangle,circle,triangle*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aNorth,Sourth,West,East*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1:5*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is {a} + {b}?</t>
+  </si>
+  <si>
     <t xml:space="preserve">numberline</t>
   </si>
   <si>
-    <t xml:space="preserve">a1:3*b1:3*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a}-{b}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a:3:9*b2:9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*b1:9*c1:9*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} - {b} -{c}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} * {b} *{c}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} /{b} /{c}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*;2/b1:9;2/c2*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} + {b} +{c}+{d}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*b1:9*c1:9*d1:9*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} - {b} -{c}+{d}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} * {b} *{c}+{d}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*b1:9*c1:9d1:9*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{a} /{b} /{c}/{d}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*;2/b1:9;2/c1:9;2d1*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*;2/b1:9;2/c1:9;2d1:2*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">angle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a60,30,45,90,120,180,270,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sterio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:9*b1:9*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drawing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arectangle,circle,triangle*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aNorth,Sourth,West,East*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">touch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a1:5*</t>
+    <t xml:space="preserve">a1:5*b1:3*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is {a} - {b}?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a3:7*b1:3*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start at {a}. Add {b}. Where?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a0:5*b1:4*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move {b} units left from {a}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a3:6*b1:2*</t>
   </si>
   <si>
     <t xml:space="preserve">You have ₹{a}, and your friend gives you ₹{b} more.</t>
@@ -417,8 +435,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,7 +631,7 @@
     </row>
     <row r="10" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>18</v>
@@ -625,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>30</v>
@@ -639,7 +657,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -653,7 +671,7 @@
     </row>
     <row r="12" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>18</v>
@@ -662,10 +680,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>30</v>
@@ -673,19 +691,19 @@
     </row>
     <row r="13" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>30</v>
@@ -693,19 +711,19 @@
     </row>
     <row r="14" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>30</v>
@@ -713,19 +731,19 @@
     </row>
     <row r="15" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>30</v>
@@ -733,19 +751,19 @@
     </row>
     <row r="16" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>30</v>
@@ -753,19 +771,19 @@
     </row>
     <row r="17" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>30</v>
@@ -773,19 +791,19 @@
     </row>
     <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D18" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>30</v>
@@ -796,13 +814,13 @@
         <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>26</v>
@@ -813,19 +831,19 @@
     </row>
     <row r="20" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="D20" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>30</v>
@@ -833,19 +851,19 @@
     </row>
     <row r="21" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>30</v>
@@ -853,19 +871,19 @@
     </row>
     <row r="22" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>30</v>
@@ -873,19 +891,19 @@
     </row>
     <row r="23" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>30</v>
@@ -893,19 +911,19 @@
     </row>
     <row r="24" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>30</v>
@@ -913,19 +931,19 @@
     </row>
     <row r="25" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>30</v>
@@ -933,19 +951,19 @@
     </row>
     <row r="26" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>30</v>
@@ -953,19 +971,19 @@
     </row>
     <row r="27" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>30</v>
@@ -976,10 +994,10 @@
         <v>9</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -993,19 +1011,19 @@
     </row>
     <row r="29" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>30</v>
@@ -1013,99 +1031,99 @@
     </row>
     <row r="30" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>9</v>
+      <c r="A34" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>30</v>
@@ -1113,53 +1131,53 @@
     </row>
     <row r="35" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>30</v>
+      <c r="F36" s="5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>49</v>
+      <c r="A37" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
@@ -1171,61 +1189,61 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>53</v>
+      <c r="F38" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
-        <v>55</v>
+      <c r="A40" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>30</v>
@@ -1233,104 +1251,66 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>30</v>
+      <c r="D42" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F45" s="5" t="n">
+      <c r="A43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="5" t="n">
         <v>5</v>
       </c>
     </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1343,7 +1323,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F45"/>
+  <autoFilter ref="A1:F43"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fix(angle):it will now load questions from excel sheets
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -125,7 +125,7 @@
     <t xml:space="preserve">angle</t>
   </si>
   <si>
-    <t xml:space="preserve">a60,30,45,90,120,180,270,360</t>
+    <t xml:space="preserve">a60,30,45,90,120,180,270,360*</t>
   </si>
   <si>
     <t xml:space="preserve">{a}-{b}</t>
@@ -435,8 +435,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix(back button):it was previously called  naviage button now it is called back button and the learning mode is except remainder is fixed
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">{a}/100 *{b}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quickplay</t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -311,6 +314,12 @@
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -362,7 +371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,6 +401,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,8 +448,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1307,6 +1320,17 @@
       </c>
       <c r="F43" s="5" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix(quickplay):it now load quesion excel by custom mode for quickplay
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t xml:space="preserve">question</t>
   </si>
@@ -271,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -314,12 +314,6 @@
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,10 +395,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1322,15 +1312,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix(remainder):fixed the question loading problem from excel
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -243,7 +243,7 @@
     <t xml:space="preserve">Reminder when {a}/{b} =</t>
   </si>
   <si>
-    <t xml:space="preserve">reminder</t>
+    <t xml:space="preserve">remainder</t>
   </si>
   <si>
     <t xml:space="preserve">{a}%{b}</t>
@@ -438,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1272,15 +1272,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>58</v>
+      <c r="C42" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
fix(touch):fixed the garbage value seelcted first number fixed that issue it basically first number was answer before now first and second number both are questions
</commit_message>
<xml_diff>
--- a/app/src/main/assets/questions/en.xlsx
+++ b/app/src/main/assets/questions/en.xlsx
@@ -2266,7 +2266,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C345" activeCellId="0" sqref="C345:C363"/>
+      <selection pane="topLeft" activeCell="A344" activeCellId="0" sqref="A344:A363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9141,7 +9141,7 @@
     </row>
     <row r="344" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>186</v>
@@ -9153,7 +9153,7 @@
         <v>1</v>
       </c>
       <c r="E344" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F344" s="3" t="n">
         <v>30</v>
@@ -9161,7 +9161,7 @@
     </row>
     <row r="345" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>186</v>
@@ -9173,7 +9173,7 @@
         <v>1</v>
       </c>
       <c r="E345" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F345" s="3" t="n">
         <v>30</v>
@@ -9181,7 +9181,7 @@
     </row>
     <row r="346" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>186</v>
@@ -9193,7 +9193,7 @@
         <v>1</v>
       </c>
       <c r="E346" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F346" s="3" t="n">
         <v>30</v>
@@ -9201,7 +9201,7 @@
     </row>
     <row r="347" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>186</v>
@@ -9213,7 +9213,7 @@
         <v>1</v>
       </c>
       <c r="E347" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F347" s="3" t="n">
         <v>30</v>
@@ -9221,7 +9221,7 @@
     </row>
     <row r="348" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>186</v>
@@ -9233,7 +9233,7 @@
         <v>1</v>
       </c>
       <c r="E348" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F348" s="3" t="n">
         <v>30</v>
@@ -9241,7 +9241,7 @@
     </row>
     <row r="349" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>186</v>
@@ -9253,7 +9253,7 @@
         <v>1</v>
       </c>
       <c r="E349" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F349" s="3" t="n">
         <v>30</v>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="350" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>186</v>
@@ -9273,7 +9273,7 @@
         <v>1</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F350" s="3" t="n">
         <v>30</v>
@@ -9281,7 +9281,7 @@
     </row>
     <row r="351" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>186</v>
@@ -9293,7 +9293,7 @@
         <v>1</v>
       </c>
       <c r="E351" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F351" s="3" t="n">
         <v>30</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="352" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>186</v>
@@ -9313,7 +9313,7 @@
         <v>1</v>
       </c>
       <c r="E352" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F352" s="3" t="n">
         <v>30</v>
@@ -9321,7 +9321,7 @@
     </row>
     <row r="353" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>186</v>
@@ -9333,7 +9333,7 @@
         <v>1</v>
       </c>
       <c r="E353" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F353" s="3" t="n">
         <v>30</v>
@@ -9341,7 +9341,7 @@
     </row>
     <row r="354" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>186</v>
@@ -9353,7 +9353,7 @@
         <v>2</v>
       </c>
       <c r="E354" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F354" s="3" t="n">
         <v>30</v>
@@ -9361,7 +9361,7 @@
     </row>
     <row r="355" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>186</v>
@@ -9373,7 +9373,7 @@
         <v>2</v>
       </c>
       <c r="E355" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F355" s="3" t="n">
         <v>30</v>
@@ -9381,7 +9381,7 @@
     </row>
     <row r="356" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>186</v>
@@ -9393,7 +9393,7 @@
         <v>2</v>
       </c>
       <c r="E356" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F356" s="3" t="n">
         <v>30</v>
@@ -9401,7 +9401,7 @@
     </row>
     <row r="357" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>186</v>
@@ -9413,7 +9413,7 @@
         <v>2</v>
       </c>
       <c r="E357" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F357" s="3" t="n">
         <v>30</v>
@@ -9421,7 +9421,7 @@
     </row>
     <row r="358" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B358" s="2" t="s">
         <v>186</v>
@@ -9433,7 +9433,7 @@
         <v>2</v>
       </c>
       <c r="E358" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F358" s="3" t="n">
         <v>30</v>
@@ -9441,7 +9441,7 @@
     </row>
     <row r="359" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B359" s="2" t="s">
         <v>186</v>
@@ -9453,7 +9453,7 @@
         <v>2</v>
       </c>
       <c r="E359" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F359" s="3" t="n">
         <v>30</v>
@@ -9461,7 +9461,7 @@
     </row>
     <row r="360" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B360" s="2" t="s">
         <v>186</v>
@@ -9473,7 +9473,7 @@
         <v>2</v>
       </c>
       <c r="E360" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F360" s="3" t="n">
         <v>30</v>
@@ -9481,7 +9481,7 @@
     </row>
     <row r="361" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B361" s="2" t="s">
         <v>186</v>
@@ -9493,7 +9493,7 @@
         <v>2</v>
       </c>
       <c r="E361" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F361" s="3" t="n">
         <v>30</v>
@@ -9501,7 +9501,7 @@
     </row>
     <row r="362" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B362" s="2" t="s">
         <v>186</v>
@@ -9513,7 +9513,7 @@
         <v>2</v>
       </c>
       <c r="E362" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F362" s="3" t="n">
         <v>30</v>
@@ -9521,7 +9521,7 @@
     </row>
     <row r="363" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>186</v>
@@ -9533,7 +9533,7 @@
         <v>2</v>
       </c>
       <c r="E363" s="2" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F363" s="3" t="n">
         <v>30</v>
@@ -21139,7 +21139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="944" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="944" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="2" t="s">
         <v>6</v>
       </c>
@@ -21159,7 +21159,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="945" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="945" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="2" t="s">
         <v>632</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="946" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="946" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="2" t="s">
         <v>633</v>
       </c>
@@ -21199,7 +21199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="947" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="947" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="2" t="s">
         <v>634</v>
       </c>
@@ -21219,7 +21219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="948" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="948" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="2" t="s">
         <v>635</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="949" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="949" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A949" s="2" t="s">
         <v>636</v>
       </c>
@@ -21259,7 +21259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="950" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="950" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A950" s="2" t="s">
         <v>637</v>
       </c>
@@ -21279,7 +21279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="951" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="951" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A951" s="2" t="s">
         <v>639</v>
       </c>
@@ -21299,7 +21299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="952" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="952" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A952" s="2" t="s">
         <v>641</v>
       </c>
@@ -21319,7 +21319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="953" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="953" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A953" s="2" t="s">
         <v>643</v>
       </c>
@@ -21339,7 +21339,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="954" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="954" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A954" s="2" t="s">
         <v>6</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="955" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="955" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A955" s="2" t="s">
         <v>632</v>
       </c>
@@ -21379,7 +21379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="956" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="956" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="2" t="s">
         <v>633</v>
       </c>
@@ -21399,7 +21399,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="957" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="957" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="2" t="s">
         <v>634</v>
       </c>
@@ -21419,7 +21419,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="958" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="958" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="2" t="s">
         <v>635</v>
       </c>
@@ -21439,7 +21439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="959" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="959" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="2" t="s">
         <v>636</v>
       </c>
@@ -21459,7 +21459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="960" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="960" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="2" t="s">
         <v>637</v>
       </c>
@@ -21479,7 +21479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="961" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="961" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A961" s="2" t="s">
         <v>639</v>
       </c>
@@ -21499,7 +21499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="962" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="962" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="2" t="s">
         <v>641</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="963" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="963" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="2" t="s">
         <v>643</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="964" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="964" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="2" t="s">
         <v>6</v>
       </c>
@@ -21559,7 +21559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="965" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="965" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="2" t="s">
         <v>632</v>
       </c>
@@ -21579,7 +21579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="966" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="966" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="2" t="s">
         <v>633</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="967" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="967" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="2" t="s">
         <v>634</v>
       </c>
@@ -21619,7 +21619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="968" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="968" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A968" s="2" t="s">
         <v>635</v>
       </c>
@@ -21639,7 +21639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="969" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="969" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A969" s="2" t="s">
         <v>636</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="970" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="970" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="2" t="s">
         <v>637</v>
       </c>
@@ -21679,7 +21679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="971" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="971" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="2" t="s">
         <v>639</v>
       </c>
@@ -21699,7 +21699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="972" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="972" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="2" t="s">
         <v>641</v>
       </c>
@@ -21719,7 +21719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="973" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="973" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A973" s="2" t="s">
         <v>643</v>
       </c>
@@ -21739,7 +21739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="974" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="974" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="2" t="s">
         <v>6</v>
       </c>
@@ -21759,7 +21759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="975" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="975" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="2" t="s">
         <v>632</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="976" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="976" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="2" t="s">
         <v>633</v>
       </c>
@@ -21799,7 +21799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="977" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="977" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="2" t="s">
         <v>634</v>
       </c>
@@ -21819,7 +21819,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="978" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="978" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="2" t="s">
         <v>635</v>
       </c>
@@ -21839,7 +21839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="979" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="979" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A979" s="2" t="s">
         <v>636</v>
       </c>
@@ -21859,7 +21859,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="980" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="980" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="2" t="s">
         <v>637</v>
       </c>
@@ -21879,7 +21879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="981" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="981" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A981" s="2" t="s">
         <v>639</v>
       </c>
@@ -21899,7 +21899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="982" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="982" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="2" t="s">
         <v>641</v>
       </c>
@@ -21919,7 +21919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="983" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="983" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A983" s="2" t="s">
         <v>643</v>
       </c>
@@ -21939,7 +21939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="984" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="984" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A984" s="2" t="s">
         <v>6</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="985" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="985" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="2" t="s">
         <v>632</v>
       </c>
@@ -21979,7 +21979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="986" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="986" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A986" s="2" t="s">
         <v>633</v>
       </c>
@@ -21999,7 +21999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="987" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="987" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A987" s="2" t="s">
         <v>634</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="988" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="988" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A988" s="2" t="s">
         <v>635</v>
       </c>
@@ -22039,7 +22039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="989" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="989" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A989" s="2" t="s">
         <v>636</v>
       </c>
@@ -22059,7 +22059,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="990" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="990" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A990" s="2" t="s">
         <v>637</v>
       </c>
@@ -22079,7 +22079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="991" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="991" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="2" t="s">
         <v>639</v>
       </c>
@@ -22099,7 +22099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="992" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="992" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="2" t="s">
         <v>641</v>
       </c>
@@ -22119,7 +22119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="993" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="993" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="2" t="s">
         <v>643</v>
       </c>
@@ -23300,6 +23300,7 @@
   <autoFilter ref="A1:F1043">
     <filterColumn colId="1">
       <filters>
+        <filter val="story"/>
         <filter val="touch"/>
       </filters>
     </filterColumn>
@@ -23323,7 +23324,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="1" sqref="C345:C363 E43"/>
+      <selection pane="topLeft" activeCell="E43" activeCellId="1" sqref="A344:A363 E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>